<commit_message>
Ultimos cambios materias primas.
</commit_message>
<xml_diff>
--- a/Robot Facturación Materia Prima/Config/Descargas/Pedidos SAP.xlsx
+++ b/Robot Facturación Materia Prima/Config/Descargas/Pedidos SAP.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="96">
   <si>
     <t>PEDIDOS DE COMPRA MATERIA PRIMA SAP</t>
   </si>
@@ -1474,8 +1474,8 @@
   </sheetPr>
   <dimension ref="A1:AA983"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B40" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4:J27"/>
+    <sheetView showGridLines="0" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1754,7 +1754,7 @@
         <v>7</v>
       </c>
       <c r="C7" s="55">
-        <v>1900003262</v>
+        <v>4400154653</v>
       </c>
       <c r="D7" s="56" t="s">
         <v>17</v>
@@ -1763,11 +1763,9 @@
         <v>18</v>
       </c>
       <c r="F7" s="61" t="s">
-        <v>22</v>
-      </c>
-      <c r="G7" s="61" t="s">
         <v>12</v>
       </c>
+      <c r="G7" s="61"/>
       <c r="H7" s="35">
         <v>0.01</v>
       </c>
@@ -29470,7 +29468,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4:E8"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>